<commit_message>
change book fields order in admin panel
</commit_message>
<xml_diff>
--- a/dbs/BeitMidrashCatalog.xlsx
+++ b/dbs/BeitMidrashCatalog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shai grossman\PycharmProjects\LibraryTrackerBackEnd\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shai grossman\PycharmProjects\LibraryTrackerBackEnd\dbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AD09B1-A720-4624-A04B-EE6B5CCAF171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED7170-3C29-4B3E-8B8C-89FFCB0CD9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,7 +1376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1392,6 +1392,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1450,7 +1457,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1669,11 +1676,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M427"/>
+  <dimension ref="A1:M430"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E427" sqref="E427"/>
+      <selection pane="bottomLeft" activeCell="A428" sqref="A428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9030,7 +9037,7 @@
       <c r="G348" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H348" s="10">
+      <c r="H348" s="5">
         <v>4</v>
       </c>
       <c r="J348" s="3">
@@ -9053,7 +9060,7 @@
       <c r="G349" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H349" s="10">
+      <c r="H349" s="5">
         <v>4</v>
       </c>
       <c r="J349" s="3">
@@ -9076,7 +9083,7 @@
       <c r="G350" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H350" s="10">
+      <c r="H350" s="5">
         <v>4</v>
       </c>
       <c r="J350" s="3">
@@ -9099,7 +9106,7 @@
       <c r="G351" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H351" s="10">
+      <c r="H351" s="5">
         <v>4</v>
       </c>
       <c r="J351" s="3">
@@ -9122,7 +9129,7 @@
       <c r="G352" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H352" s="10">
+      <c r="H352" s="5">
         <v>4</v>
       </c>
       <c r="J352" s="3">
@@ -9145,7 +9152,7 @@
       <c r="G353" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H353" s="10">
+      <c r="H353" s="5">
         <v>4</v>
       </c>
       <c r="J353" s="3">
@@ -10770,6 +10777,22 @@
       <c r="H427" s="5">
         <v>7</v>
       </c>
+    </row>
+    <row r="429" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A429" s="3"/>
+      <c r="D429" s="3"/>
+      <c r="E429" s="3"/>
+      <c r="F429" s="10"/>
+      <c r="G429" s="3"/>
+      <c r="H429" s="3"/>
+    </row>
+    <row r="430" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A430" s="10"/>
+      <c r="D430" s="10"/>
+      <c r="E430" s="3"/>
+      <c r="F430" s="3"/>
+      <c r="G430" s="3"/>
+      <c r="H430" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10778,5 +10801,6 @@
     <mergeCell ref="K292:K296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>